<commit_message>
added script for acquiring ensembl ids from gene name
</commit_message>
<xml_diff>
--- a/left_associated.xlsx
+++ b/left_associated.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,281 +441,1181 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>BRAF</t>
+          <t>AURKB</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.001649563643547397</v>
+        <v>3.654969382948658</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>IGF1R</t>
+          <t>AXIN1</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.02129755716279117</v>
+        <v>1.107504460543004</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>KMT2D</t>
+          <t>EPHB4</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.002765832806025661</v>
+        <v>1.218624438666982</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>RAD21</t>
+          <t>FGF23</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.005868839624676088</v>
+        <v>2.132838283828383</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>RNF43</t>
+          <t>H3-3A</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.499018300941508e-05</v>
+        <v>1.624185316058108</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>APC</t>
+          <t>MRE11</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.329580677006993e-36</v>
+        <v>1.043803238948183</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>KRAS</t>
+          <t>NTRK2</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>5.715203832289061e-09</v>
+        <v>1.462544253009205</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>TP53</t>
+          <t>PIK3CA</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1.927707070267472e-29</v>
+        <v>1.290509550138226</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>CREBBP</t>
+          <t>RET</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.01289220685475154</v>
+        <v>1.025526253621296</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>SMAD4</t>
+          <t>SOX9</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.0008281868150068861</v>
+        <v>1.024721200841315</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>ACVR1B</t>
+          <t>SYK</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.005033609400641829</v>
+        <v>1.217954759660697</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>FBXW7</t>
+          <t>TYRO3</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.003296128576176917</v>
+        <v>2.074385633270321</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>BCOR</t>
+          <t>APC</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01100811959142297</v>
+        <v>2.553218217665156</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>RPTOR</t>
+          <t>KLHL6</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.04438291628599782</v>
+        <v>1.065594059405941</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>CIC</t>
+          <t>KRAS</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.02173798681211427</v>
+        <v>1.958937409488041</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>POLD1</t>
+          <t>TP53</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01234775778938848</v>
+        <v>2.764803865749865</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>POLE</t>
+          <t>ATM</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.04076564471113148</v>
+        <v>1.135440384694423</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>HNF1A</t>
+          <t>FGF12</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1.119406325078457e-05</v>
+        <v>1.218057520037718</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>WT1</t>
+          <t>SMAD4</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.01913417133249251</v>
+        <v>1.819425566127413</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>ASXL1</t>
+          <t>CUL3</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.006171715730209176</v>
+        <v>2.132838283828383</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>TNFAIP3</t>
+          <t>XPO1</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.006341753666897882</v>
+        <v>1.082553905001441</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>SMARCB1</t>
+          <t>CEBPA</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.02745472385955084</v>
+        <v>1.217954759660697</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>NF1</t>
+          <t>DNMT3A</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.01045697321053559</v>
+        <v>1.124733727810651</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>TENT5C</t>
+          <t>FBXW7</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.01861770695010301</v>
+        <v>1.747657132391099</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>BARD1</t>
+          <t>KDM6A</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.02493501298981447</v>
+        <v>1.218417945690673</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>AKT1</t>
+          <t>KEAP1</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.005868839624676088</v>
+        <v>1.218108936571563</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>PPP2R1A</t>
+          <t>MAP2K1</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.008991663889493393</v>
+        <v>1.950106107050224</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>CTNNA1</t>
+          <t>NRAS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.0006854739217738071</v>
+        <v>2.074385633270321</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>RAF1</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1.218211842415664</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>ERBB2</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1.402531945101751</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>AR</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1.082709924665984</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>MED12</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1.087746888528139</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>BAP1</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1.107250852473783</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>BRCA2</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1.014906438312718</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>CDC73</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1.950106107050224</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>KDR</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2.034365886340348</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>MYC</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1.217852096090438</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>PRKAR1A</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>1.217903415783274</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>FANCC</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>1.461890172048079</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>ERRFI1</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>7.315107235446618</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>KEL</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2.643374252439408</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>NSD3</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1.448020094562648</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>DDR1</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1.116525090451471</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>MAP2K4</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1.218676122931442</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>MUTYH</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>1.462544253009205</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>HSD3B1</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.624185316058108</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
+          <t>DIS3</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>1.422038567493113</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>MITF</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>1.107250852473783</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>CD79B</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>FGF4</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>6.094486333647502</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="inlineStr">
+        <is>
+          <t>JUN</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>3.251434410123399</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="inlineStr">
+        <is>
+          <t>LTK</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>1.218006127739807</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="inlineStr">
+        <is>
+          <t>MAP3K1</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>1.136969696969697</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>PRKCI</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>1.218006127739807</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="inlineStr">
+        <is>
+          <t>ZNF217</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>1.353830830122408</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="inlineStr">
+        <is>
+          <t>IRF2</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>1.461890172048079</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="inlineStr">
+        <is>
+          <t>TEK</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>1.014783360855548</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="inlineStr">
+        <is>
+          <t>GABRA6</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>1.065594059405941</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="inlineStr">
+        <is>
+          <t>PIK3C2G</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.142093764761455</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="inlineStr">
+        <is>
+          <t>FGF14</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>1.62477403128193</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>PRDM1</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1.625363858075682</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="inlineStr">
+        <is>
+          <t>MTOR</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>1.124733727810651</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="inlineStr">
+        <is>
+          <t>FGFR2</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1.218263331760264</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="inlineStr">
+        <is>
+          <t>RAD51</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>7.315107235446618</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>XRCC2</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>3.046654099905749</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="inlineStr">
+        <is>
+          <t>ARAF</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>1.096132075471698</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="inlineStr">
+        <is>
+          <t>EPHB1</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>1.218831322450911</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="inlineStr">
+        <is>
+          <t>IDH1</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>1.065594059405941</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="inlineStr">
+        <is>
+          <t>MYD88</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>3.654969382948658</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="inlineStr">
+        <is>
+          <t>NTRK3</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>1.402531945101751</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>SDHD</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>3.654969382948658</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="inlineStr">
+        <is>
+          <t>TGFBR2</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1.030438886267107</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="inlineStr">
+        <is>
+          <t>ALK</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1.497609922053314</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="inlineStr">
+        <is>
+          <t>CTNNB1</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>1.179686365061282</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>SUFU</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>1.522737983034873</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="inlineStr">
+        <is>
+          <t>SF3B1</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>1.065702479338843</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="inlineStr">
+        <is>
+          <t>PDK1</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>3.046654099905749</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="inlineStr">
+        <is>
+          <t>AURKA</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="inlineStr">
+        <is>
+          <t>BTG2</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>FANCL</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>1.218006127739807</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="inlineStr">
+        <is>
+          <t>FGF19</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="inlineStr">
+        <is>
+          <t>MAP3K13</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>1.741313652141678</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="inlineStr">
+        <is>
+          <t>NT5C2</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>1.392393977161721</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="inlineStr">
+        <is>
+          <t>ROS1</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>1.335485543010389</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="inlineStr">
+        <is>
+          <t>CHEK1</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>4.267326732673268</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="inlineStr">
+        <is>
+          <t>SMAD2</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1.320152659741895</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="inlineStr">
+        <is>
+          <t>FGF3</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>1.218006127739807</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>IRF4</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>1.522737983034873</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="inlineStr">
+        <is>
+          <t>IKZF1</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>1.014783360855548</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>1.353830830122408</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="inlineStr">
+        <is>
+          <t>JAK2</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>1.218263331760264</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="inlineStr">
+        <is>
+          <t>AKT3</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>1.014765944077914</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="inlineStr">
+        <is>
+          <t>PMS2</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>1.218211842415664</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>SDHB</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="inlineStr">
+        <is>
+          <t>CD22</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>1.218211842415664</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="inlineStr">
+        <is>
+          <t>DDR2</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>1.107250852473783</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="inlineStr">
+        <is>
+          <t>GNAQ</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>2.436749116607774</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="inlineStr">
+        <is>
+          <t>CDKN1B</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1.624185316058108</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="inlineStr">
+        <is>
+          <t>PTPN11</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>1.065594059405941</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>CCND3</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>1.217749529190207</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="inlineStr">
+        <is>
+          <t>GNA13</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>3.654969382948658</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="inlineStr">
+        <is>
+          <t>TIPARP</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>1.522737983034873</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="inlineStr">
+        <is>
+          <t>MDM2</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>2.43607252178008</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="inlineStr">
+        <is>
+          <t>MKNK1</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>1.217852096090438</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="inlineStr">
+        <is>
+          <t>BCL2L1</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>1.217800800565105</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="inlineStr">
+        <is>
+          <t>IDH2</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>1.014765944077914</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>RAD54L</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>2.030710021991831</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="inlineStr">
+        <is>
+          <t>CDKN1A</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>2.43607252178008</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="inlineStr">
+        <is>
+          <t>HDAC1</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>1.082553905001441</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="inlineStr">
+        <is>
+          <t>RAC1</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>2.43607252178008</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="1" t="inlineStr">
+        <is>
+          <t>ARFRP1</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>1.827131417804993</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="1" t="inlineStr">
+        <is>
+          <t>FLT3</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1.392393977161721</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="1" t="inlineStr">
+        <is>
+          <t>MEF2B</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>2.43607252178008</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>PIM1</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>1.827131417804993</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="1" t="inlineStr">
+        <is>
+          <t>CDK4</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>1.217749529190207</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="1" t="inlineStr">
+        <is>
+          <t>RAD52</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>1.827131417804993</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="1" t="inlineStr">
+        <is>
+          <t>SDHC</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>1.217749529190207</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="1" t="inlineStr">
+        <is>
+          <t>TERT</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>1.827716238510488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>